<commit_message>
entrega de fase 3
</commit_message>
<xml_diff>
--- a/Base de datos/Diccionario de Datos IdHand.xlsx
+++ b/Base de datos/Diccionario de Datos IdHand.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\IdHand\Base de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Entrega fase 3\Base de datos  IdHand - Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="106">
   <si>
     <t>Descripción</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Es la contraseña del administrador.</t>
   </si>
   <si>
-    <t xml:space="preserve">varchar(12) </t>
-  </si>
-  <si>
     <t>Contiene las claves foráneas de la entidad Administrador y Usuario.</t>
   </si>
   <si>
@@ -306,6 +303,45 @@
   </si>
   <si>
     <t>varchar(3)</t>
+  </si>
+  <si>
+    <t>Varchar(12)</t>
+  </si>
+  <si>
+    <t>Nombre del administrador</t>
+  </si>
+  <si>
+    <t>Fecha_Admin</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>Fecha de modificación</t>
+  </si>
+  <si>
+    <t>Telefono_CentroR</t>
+  </si>
+  <si>
+    <t>Fecha_padecimiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de cuando le empezo la enfermedad </t>
+  </si>
+  <si>
+    <t>Fecha_Contacto</t>
+  </si>
+  <si>
+    <t>Fecha de cuando ingreso el número del contacto</t>
+  </si>
+  <si>
+    <t>Es el teléfono del centron de remisión</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -499,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -588,10 +624,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -605,6 +641,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,8 +961,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla24523710111314" displayName="Tabla24523710111314" ref="A74:E77" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A74:E77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla24523710111314" displayName="Tabla24523710111314" ref="A79:E82" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A79:E82"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Campo" dataDxfId="4"/>
     <tableColumn id="2" name="Tipo" dataDxfId="3"/>
@@ -947,8 +989,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla2452" displayName="Tabla2452" ref="A30:E32" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
-  <autoFilter ref="A30:E32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla2452" displayName="Tabla2452" ref="A30:E34" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A30:E34"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Campo" dataDxfId="53"/>
     <tableColumn id="2" name="Tipo" dataDxfId="52"/>
@@ -961,8 +1003,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla24523" displayName="Tabla24523" ref="A36:E38" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
-  <autoFilter ref="A36:E38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla24523" displayName="Tabla24523" ref="A38:E41" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A38:E41"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Campo" dataDxfId="46"/>
     <tableColumn id="2" name="Tipo" dataDxfId="45"/>
@@ -975,8 +1017,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla2452378" displayName="Tabla2452378" ref="A42:E44" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="A42:E44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla2452378" displayName="Tabla2452378" ref="A45:E47" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A45:E47"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Campo" dataDxfId="39"/>
     <tableColumn id="2" name="Tipo" dataDxfId="38"/>
@@ -989,8 +1031,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla2452379" displayName="Tabla2452379" ref="A48:E51" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A48:E51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla2452379" displayName="Tabla2452379" ref="A51:E54" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="A51:E54"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Campo" dataDxfId="32"/>
     <tableColumn id="2" name="Tipo" dataDxfId="31"/>
@@ -1003,8 +1045,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla24523710" displayName="Tabla24523710" ref="A55:E57" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A55:E57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla24523710" displayName="Tabla24523710" ref="A58:E61" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A58:E61"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Campo" dataDxfId="25"/>
     <tableColumn id="2" name="Tipo" dataDxfId="24"/>
@@ -1017,8 +1059,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla2452371011" displayName="Tabla2452371011" ref="A61:E63" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A61:E63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla2452371011" displayName="Tabla2452371011" ref="A65:E68" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A65:E68"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Campo" dataDxfId="18"/>
     <tableColumn id="2" name="Tipo" dataDxfId="17"/>
@@ -1031,8 +1073,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla245237101113" displayName="Tabla245237101113" ref="A67:E70" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A67:E70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla245237101113" displayName="Tabla245237101113" ref="A72:E75" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A72:E75"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Campo" dataDxfId="11"/>
     <tableColumn id="2" name="Tipo" dataDxfId="10"/>
@@ -1307,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,12 +1388,12 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -1386,7 +1428,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>4</v>
@@ -1455,7 +1497,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>6</v>
@@ -1540,7 +1582,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>6</v>
@@ -1549,7 +1591,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1570,12 +1612,12 @@
       <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="31"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="37"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
@@ -1610,7 +1652,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>4</v>
@@ -1681,19 +1723,19 @@
       <c r="A28" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="32"/>
       <c r="D29" s="32"/>
@@ -1721,623 +1763,709 @@
         <v>36</v>
       </c>
       <c r="B31" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="16" t="s">
+      <c r="C32" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="37"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="33"/>
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="37"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="33"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="37"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="33"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="37"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="33"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="B59" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="B63" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="36"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="37"/>
+    </row>
+    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="33"/>
-      <c r="G35" s="12"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="B64" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="33"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B65" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C65" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D65" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E65" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G37" s="12"/>
-    </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="6" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="37"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="33"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B73" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="C74" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="31"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="B77" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
+      <c r="E77" s="37"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="33"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="B78" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="33"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B79" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C79" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D79" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="E79" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C80" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="31"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="33"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" s="21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="31"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" s="32" t="s">
+      <c r="B82" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="33"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B55" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="31"/>
-    </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="33"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B61" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C61" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B62" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E62" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B65" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C65" s="30"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="31"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B66" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="33"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C67" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E67" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B68" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C68" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D68" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E68" s="21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B69" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E69" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B72" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C72" s="30"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="31"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="33"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B74" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D74" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E74" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B75" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C75" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E75" s="21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B76" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C76" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E76" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B60:E60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>